<commit_message>
more work more work
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="STATUS" sheetId="1" r:id="rId1"/>
-    <sheet name="lab_lab1" sheetId="2" r:id="rId2"/>
-    <sheet name="lab_lab2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>lab1</t>
   </si>
@@ -27,61 +25,25 @@
     <t>przeslane/wszystkie</t>
   </si>
   <si>
+    <t>Grzegorz Pustułka 3423424</t>
+  </si>
+  <si>
+    <t>lab1:True</t>
+  </si>
+  <si>
+    <t>1/1</t>
+  </si>
+  <si>
     <t>Mateusz Jamróz 1101506</t>
   </si>
   <si>
-    <t>lab1:True</t>
-  </si>
-  <si>
     <t>lab2:True</t>
   </si>
   <si>
     <t>2/2</t>
   </si>
   <si>
-    <t>Mateusz Jamróz 1299999</t>
-  </si>
-  <si>
-    <t>1/1</t>
-  </si>
-  <si>
-    <t>Numer zadania</t>
-  </si>
-  <si>
-    <t>kto to zrobil</t>
-  </si>
-  <si>
-    <t>Czy przeszlo?</t>
-  </si>
-  <si>
-    <t>zadanie 1</t>
-  </si>
-  <si>
-    <t>Mateusz Jamróz</t>
-  </si>
-  <si>
-    <t>zadanie 2</t>
-  </si>
-  <si>
-    <t>zadanie 3</t>
-  </si>
-  <si>
-    <t>zadanie 4</t>
-  </si>
-  <si>
-    <t>zadanie 5</t>
-  </si>
-  <si>
-    <t>zadanie 6</t>
-  </si>
-  <si>
-    <t>zadanie 7</t>
-  </si>
-  <si>
-    <t>zadanie 8</t>
-  </si>
-  <si>
-    <t>zadanie 9</t>
+    <t>Grzegorz Pustulka</t>
   </si>
 </sst>
 </file>
@@ -413,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -440,243 +402,30 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>